<commit_message>
Updated Excel to CSV
</commit_message>
<xml_diff>
--- a/Sababas Thesis Dataset/data/Drugs/List of Drugs.xlsx
+++ b/Sababas Thesis Dataset/data/Drugs/List of Drugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Sababas Thesis Dataset\data\Drugs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8D52A3-7BF9-4619-8155-F5B8CD743D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AC49F7-0C5E-4ECC-A91E-FAD9463A06AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,10 +180,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -469,7 +469,7 @@
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added the Atorvastatin and updated the Drug List
</commit_message>
<xml_diff>
--- a/Sababas Thesis Dataset/data/Drugs/List of Drugs.xlsx
+++ b/Sababas Thesis Dataset/data/Drugs/List of Drugs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Deep-Learning-Projects\Sababas Thesis Dataset\data\Drugs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Deep-Learning-Projects\Sababas Thesis Dataset\data\Drugs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4474457A-1AAA-4163-826F-F65F4E9DCF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B00B75-2FB9-48FB-89D8-0D1B809FD319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,29 +469,29 @@
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -538,334 +538,334 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="1"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="1"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="1"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" s="1"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" s="1"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" s="1"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" s="1"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" s="1"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" s="1"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="1"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="1"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="1"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="1"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="1"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="1"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="1"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="1"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" s="1"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" s="1"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Only one of them is Remaining
</commit_message>
<xml_diff>
--- a/Sababas Thesis Dataset/data/Drugs/List of Drugs.xlsx
+++ b/Sababas Thesis Dataset/data/Drugs/List of Drugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Deep-Learning-Projects\Sababas Thesis Dataset\data\Drugs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B00B75-2FB9-48FB-89D8-0D1B809FD319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA1A997-656B-4856-BDA7-37A2C5B9A468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,12 +153,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -172,15 +166,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -469,7 +460,7 @@
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,43 +548,43 @@
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1"/>

</xml_diff>